<commit_message>
edited OOSTT user-centered definition: trauma center reverification
</commit_message>
<xml_diff>
--- a/TermSurveyResponses.xlsx
+++ b/TermSurveyResponses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathiasbrochhausen/OOSTT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{53810F97-DE96-F344-BE7D-4AD663B4B1FA}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EE7F35D8-5089-594C-8878-9FBE462E1372}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="460" windowWidth="27740" windowHeight="17540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="803">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="806">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -2475,6 +2475,15 @@
   </si>
   <si>
     <t>https://github.com/OOSTT/OOSTT/commit/e9c3f191a3817acbe2ac9c16b82789b5553170c0</t>
+  </si>
+  <si>
+    <t>OOSTT aims to be agnostic under which jursidiction and by whose criteria trauma center reverification is done. Hence we will not change that. We are open to consider adding a subclass "ACS trauma center reverification".</t>
+  </si>
+  <si>
+    <t>Change made as proposed</t>
+  </si>
+  <si>
+    <t>We took out the parenthesis to clarify that the definition is open to non-ACS reverifcation</t>
   </si>
 </sst>
 </file>
@@ -8854,9 +8863,9 @@
   </sheetPr>
   <dimension ref="A1:IW1418"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J80" sqref="J80"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G101" sqref="G101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10540,7 +10549,7 @@
       <c r="E75" s="45"/>
       <c r="F75" s="46"/>
       <c r="G75" s="47"/>
-      <c r="H75" s="47"/>
+      <c r="H75" s="60"/>
       <c r="I75" s="47"/>
       <c r="J75" s="47"/>
     </row>
@@ -10561,7 +10570,7 @@
       <c r="E76" s="45"/>
       <c r="F76" s="46"/>
       <c r="G76" s="47"/>
-      <c r="H76" s="47"/>
+      <c r="H76" s="60"/>
       <c r="I76" s="47"/>
       <c r="J76" s="47"/>
     </row>
@@ -10582,7 +10591,7 @@
       <c r="E77" s="45"/>
       <c r="F77" s="46"/>
       <c r="G77" s="47"/>
-      <c r="H77" s="47"/>
+      <c r="H77" s="60"/>
       <c r="I77" s="47"/>
       <c r="J77" s="47"/>
     </row>
@@ -10603,7 +10612,7 @@
       <c r="E78" s="45"/>
       <c r="F78" s="46"/>
       <c r="G78" s="47"/>
-      <c r="H78" s="47"/>
+      <c r="H78" s="60"/>
       <c r="I78" s="47"/>
       <c r="J78" s="47"/>
     </row>
@@ -10624,7 +10633,7 @@
       <c r="E79" s="45"/>
       <c r="F79" s="46"/>
       <c r="G79" s="47"/>
-      <c r="H79" s="47"/>
+      <c r="H79" s="60"/>
       <c r="I79" s="47"/>
       <c r="J79" s="47"/>
     </row>
@@ -10651,7 +10660,7 @@
       <c r="G80" s="62" t="s">
         <v>801</v>
       </c>
-      <c r="H80" s="47"/>
+      <c r="H80" s="60"/>
       <c r="I80" s="47"/>
       <c r="J80" s="62" t="s">
         <v>802</v>
@@ -10674,7 +10683,7 @@
       <c r="E81" s="45"/>
       <c r="F81" s="46"/>
       <c r="G81" s="47"/>
-      <c r="H81" s="47"/>
+      <c r="H81" s="60"/>
       <c r="I81" s="47"/>
       <c r="J81" s="47"/>
     </row>
@@ -10695,7 +10704,7 @@
       <c r="E82" s="45"/>
       <c r="F82" s="46"/>
       <c r="G82" s="47"/>
-      <c r="H82" s="47"/>
+      <c r="H82" s="60"/>
       <c r="I82" s="47"/>
       <c r="J82" s="47"/>
     </row>
@@ -10716,7 +10725,7 @@
       <c r="E83" s="45"/>
       <c r="F83" s="46"/>
       <c r="G83" s="47"/>
-      <c r="H83" s="47"/>
+      <c r="H83" s="60"/>
       <c r="I83" s="47"/>
       <c r="J83" s="47"/>
     </row>
@@ -10737,7 +10746,7 @@
       <c r="E84" s="56"/>
       <c r="F84" s="37"/>
       <c r="G84" s="36"/>
-      <c r="H84" s="36"/>
+      <c r="H84" s="60"/>
       <c r="I84" s="36"/>
       <c r="J84" s="36"/>
     </row>
@@ -10758,7 +10767,7 @@
       <c r="E85" s="56"/>
       <c r="F85" s="37"/>
       <c r="G85" s="36"/>
-      <c r="H85" s="36"/>
+      <c r="H85" s="60"/>
       <c r="I85" s="36"/>
       <c r="J85" s="36"/>
     </row>
@@ -10777,7 +10786,7 @@
       <c r="E86" s="56"/>
       <c r="F86" s="37"/>
       <c r="G86" s="36"/>
-      <c r="H86" s="36"/>
+      <c r="H86" s="60"/>
       <c r="I86" s="36"/>
       <c r="J86" s="36"/>
     </row>
@@ -10798,7 +10807,7 @@
       <c r="E87" s="56"/>
       <c r="F87" s="37"/>
       <c r="G87" s="36"/>
-      <c r="H87" s="36"/>
+      <c r="H87" s="60"/>
       <c r="I87" s="36"/>
       <c r="J87" s="36"/>
     </row>
@@ -10819,7 +10828,7 @@
       <c r="E88" s="56"/>
       <c r="F88" s="37"/>
       <c r="G88" s="36"/>
-      <c r="H88" s="36"/>
+      <c r="H88" s="60"/>
       <c r="I88" s="36"/>
       <c r="J88" s="36"/>
     </row>
@@ -10840,7 +10849,7 @@
       <c r="E89" s="56"/>
       <c r="F89" s="37"/>
       <c r="G89" s="36"/>
-      <c r="H89" s="36"/>
+      <c r="H89" s="60"/>
       <c r="I89" s="36"/>
       <c r="J89" s="36"/>
     </row>
@@ -10861,7 +10870,7 @@
       <c r="E90" s="56"/>
       <c r="F90" s="37"/>
       <c r="G90" s="36"/>
-      <c r="H90" s="36"/>
+      <c r="H90" s="60"/>
       <c r="I90" s="36"/>
       <c r="J90" s="36"/>
     </row>
@@ -10882,7 +10891,7 @@
       <c r="E91" s="56"/>
       <c r="F91" s="37"/>
       <c r="G91" s="36"/>
-      <c r="H91" s="36"/>
+      <c r="H91" s="60"/>
       <c r="I91" s="36"/>
       <c r="J91" s="36"/>
     </row>
@@ -10903,7 +10912,7 @@
       <c r="E92" s="56"/>
       <c r="F92" s="37"/>
       <c r="G92" s="36"/>
-      <c r="H92" s="36"/>
+      <c r="H92" s="60"/>
       <c r="I92" s="36"/>
       <c r="J92" s="36"/>
     </row>
@@ -10949,7 +10958,7 @@
       <c r="I94" s="47"/>
       <c r="J94" s="47"/>
     </row>
-    <row r="95" spans="1:10" ht="65" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:10" ht="104" x14ac:dyDescent="0.15">
       <c r="A95" s="19">
         <v>13</v>
       </c>
@@ -10967,7 +10976,9 @@
         <v>183</v>
       </c>
       <c r="F95" s="46"/>
-      <c r="G95" s="47"/>
+      <c r="G95" s="62" t="s">
+        <v>803</v>
+      </c>
       <c r="H95" s="47"/>
       <c r="I95" s="47"/>
       <c r="J95" s="47"/>
@@ -11053,7 +11064,9 @@
       <c r="F99" s="55" t="s">
         <v>184</v>
       </c>
-      <c r="G99" s="47"/>
+      <c r="G99" s="47" t="s">
+        <v>804</v>
+      </c>
       <c r="H99" s="47"/>
       <c r="I99" s="47"/>
       <c r="J99" s="47"/>
@@ -11076,12 +11089,14 @@
         <v>185</v>
       </c>
       <c r="F100" s="46"/>
-      <c r="G100" s="47"/>
+      <c r="G100" s="47" t="s">
+        <v>804</v>
+      </c>
       <c r="H100" s="47"/>
       <c r="I100" s="47"/>
       <c r="J100" s="47"/>
     </row>
-    <row r="101" spans="1:10" ht="26" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:10" ht="39" x14ac:dyDescent="0.15">
       <c r="A101" s="19">
         <v>13</v>
       </c>
@@ -11099,7 +11114,9 @@
       <c r="F101" s="55" t="s">
         <v>186</v>
       </c>
-      <c r="G101" s="47"/>
+      <c r="G101" s="62" t="s">
+        <v>805</v>
+      </c>
       <c r="H101" s="47"/>
       <c r="I101" s="47"/>
       <c r="J101" s="47"/>

</xml_diff>

<commit_message>
changed label of 'institution-specific emergency medicine physician profile' to 'institution-specific emergency medicine physician role description'
</commit_message>
<xml_diff>
--- a/TermSurveyResponses.xlsx
+++ b/TermSurveyResponses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathiasbrochhausen/OOSTT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EE7F35D8-5089-594C-8878-9FBE462E1372}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{78CF7CBC-6CC7-FB44-87F0-7B2BCF08F951}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="460" windowWidth="27740" windowHeight="17540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="808">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -2484,6 +2484,12 @@
   </si>
   <si>
     <t>We took out the parenthesis to clarify that the definition is open to non-ACS reverifcation</t>
+  </si>
+  <si>
+    <t>https://github.com/OOSTT/OOSTT/commit/c2220a9641cf0049edcd87f2fb0db338352c1159</t>
+  </si>
+  <si>
+    <t>A process  to determine whether a verified trauma center continues to meet the verification standards of the American College of Surgeons or a similar process in a particular trauma system or jurisdiction within a specified time period.</t>
   </si>
 </sst>
 </file>
@@ -8863,9 +8869,9 @@
   </sheetPr>
   <dimension ref="A1:IW1418"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G101" sqref="G101"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I101" sqref="I101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10933,7 +10939,7 @@
       <c r="E93" s="45"/>
       <c r="F93" s="46"/>
       <c r="G93" s="47"/>
-      <c r="H93" s="47"/>
+      <c r="H93" s="60"/>
       <c r="I93" s="47"/>
       <c r="J93" s="47"/>
     </row>
@@ -10954,7 +10960,7 @@
       <c r="E94" s="45"/>
       <c r="F94" s="46"/>
       <c r="G94" s="47"/>
-      <c r="H94" s="47"/>
+      <c r="H94" s="60"/>
       <c r="I94" s="47"/>
       <c r="J94" s="47"/>
     </row>
@@ -10979,7 +10985,7 @@
       <c r="G95" s="62" t="s">
         <v>803</v>
       </c>
-      <c r="H95" s="47"/>
+      <c r="H95" s="60"/>
       <c r="I95" s="47"/>
       <c r="J95" s="47"/>
     </row>
@@ -11000,7 +11006,7 @@
       <c r="E96" s="45"/>
       <c r="F96" s="46"/>
       <c r="G96" s="47"/>
-      <c r="H96" s="47"/>
+      <c r="H96" s="60"/>
       <c r="I96" s="47"/>
       <c r="J96" s="47"/>
     </row>
@@ -11021,7 +11027,7 @@
       <c r="E97" s="45"/>
       <c r="F97" s="46"/>
       <c r="G97" s="47"/>
-      <c r="H97" s="47"/>
+      <c r="H97" s="60"/>
       <c r="I97" s="47"/>
       <c r="J97" s="47"/>
     </row>
@@ -11042,7 +11048,7 @@
       <c r="E98" s="45"/>
       <c r="F98" s="46"/>
       <c r="G98" s="47"/>
-      <c r="H98" s="47"/>
+      <c r="H98" s="60"/>
       <c r="I98" s="47"/>
       <c r="J98" s="47"/>
     </row>
@@ -11067,11 +11073,13 @@
       <c r="G99" s="47" t="s">
         <v>804</v>
       </c>
-      <c r="H99" s="47"/>
-      <c r="I99" s="47"/>
-      <c r="J99" s="47"/>
-    </row>
-    <row r="100" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+      <c r="H99" s="60"/>
+      <c r="I99" s="62"/>
+      <c r="J99" s="62" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" ht="39" x14ac:dyDescent="0.15">
       <c r="A100" s="19">
         <v>13</v>
       </c>
@@ -11092,11 +11100,13 @@
       <c r="G100" s="47" t="s">
         <v>804</v>
       </c>
-      <c r="H100" s="47"/>
-      <c r="I100" s="47"/>
-      <c r="J100" s="47"/>
-    </row>
-    <row r="101" spans="1:10" ht="39" x14ac:dyDescent="0.15">
+      <c r="H100" s="60"/>
+      <c r="I100" s="62"/>
+      <c r="J100" s="62" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" ht="65" x14ac:dyDescent="0.15">
       <c r="A101" s="19">
         <v>13</v>
       </c>
@@ -11117,9 +11127,13 @@
       <c r="G101" s="62" t="s">
         <v>805</v>
       </c>
-      <c r="H101" s="47"/>
-      <c r="I101" s="47"/>
-      <c r="J101" s="47"/>
+      <c r="H101" s="60"/>
+      <c r="I101" s="62" t="s">
+        <v>807</v>
+      </c>
+      <c r="J101" s="62" t="s">
+        <v>806</v>
+      </c>
     </row>
     <row r="102" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A102" s="19">
@@ -11138,7 +11152,7 @@
       <c r="E102" s="45"/>
       <c r="F102" s="46"/>
       <c r="G102" s="47"/>
-      <c r="H102" s="47"/>
+      <c r="H102" s="60"/>
       <c r="I102" s="47"/>
       <c r="J102" s="47"/>
     </row>

</xml_diff>

<commit_message>
added label 'head of emergency medicine role' to 'head of emergency medicine department role.
</commit_message>
<xml_diff>
--- a/TermSurveyResponses.xlsx
+++ b/TermSurveyResponses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathiasbrochhausen/OOSTT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AF14936A-FEBD-FC44-861F-F5B0B862FE8D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{73C316DE-2688-7644-9AFD-A02BCA3AE3C3}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="460" windowWidth="27740" windowHeight="17540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="812">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="813">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -2503,6 +2503,9 @@
   <si>
     <t>https://github.com/OOSTT/OOSTT/commit/2ce41519b9b284758de2b5903821c61d28451687
 https://github.com/OOSTT/OOSTT/commit/9ae880f66b9db0e452a0f7e2ec4bf759bac54c28</t>
+  </si>
+  <si>
+    <t>Since this is the only comment that indicates that this is a problem and we are following the phrazing of the ACS' "Resources for optimal trauma care"</t>
   </si>
 </sst>
 </file>
@@ -8882,9 +8885,9 @@
   </sheetPr>
   <dimension ref="A1:IW1418"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I103" sqref="I103"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H121" sqref="H121:H129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -11586,7 +11589,7 @@
       <c r="E121" s="56"/>
       <c r="F121" s="37"/>
       <c r="G121" s="36"/>
-      <c r="H121" s="36"/>
+      <c r="H121" s="60"/>
       <c r="I121" s="36"/>
       <c r="J121" s="36"/>
     </row>
@@ -11607,7 +11610,7 @@
       <c r="E122" s="56"/>
       <c r="F122" s="37"/>
       <c r="G122" s="36"/>
-      <c r="H122" s="36"/>
+      <c r="H122" s="60"/>
       <c r="I122" s="36"/>
       <c r="J122" s="36"/>
     </row>
@@ -11626,7 +11629,7 @@
       <c r="E123" s="56"/>
       <c r="F123" s="37"/>
       <c r="G123" s="36"/>
-      <c r="H123" s="36"/>
+      <c r="H123" s="60"/>
       <c r="I123" s="36"/>
       <c r="J123" s="36"/>
     </row>
@@ -11647,7 +11650,7 @@
       <c r="E124" s="56"/>
       <c r="F124" s="37"/>
       <c r="G124" s="36"/>
-      <c r="H124" s="36"/>
+      <c r="H124" s="60"/>
       <c r="I124" s="36"/>
       <c r="J124" s="36"/>
     </row>
@@ -11668,7 +11671,7 @@
       <c r="E125" s="56"/>
       <c r="F125" s="37"/>
       <c r="G125" s="36"/>
-      <c r="H125" s="36"/>
+      <c r="H125" s="60"/>
       <c r="I125" s="36"/>
       <c r="J125" s="36"/>
     </row>
@@ -11689,7 +11692,7 @@
       <c r="E126" s="56"/>
       <c r="F126" s="37"/>
       <c r="G126" s="36"/>
-      <c r="H126" s="36"/>
+      <c r="H126" s="60"/>
       <c r="I126" s="36"/>
       <c r="J126" s="36"/>
     </row>
@@ -11710,7 +11713,7 @@
       <c r="E127" s="56"/>
       <c r="F127" s="37"/>
       <c r="G127" s="36"/>
-      <c r="H127" s="36"/>
+      <c r="H127" s="60"/>
       <c r="I127" s="36"/>
       <c r="J127" s="36"/>
     </row>
@@ -11731,9 +11734,11 @@
       <c r="E128" s="32" t="s">
         <v>191</v>
       </c>
-      <c r="F128" s="37"/>
+      <c r="F128" s="37" t="s">
+        <v>812</v>
+      </c>
       <c r="G128" s="36"/>
-      <c r="H128" s="36"/>
+      <c r="H128" s="60"/>
       <c r="I128" s="36"/>
       <c r="J128" s="36"/>
     </row>
@@ -11754,7 +11759,7 @@
       <c r="E129" s="56"/>
       <c r="F129" s="37"/>
       <c r="G129" s="36"/>
-      <c r="H129" s="36"/>
+      <c r="H129" s="60"/>
       <c r="I129" s="36"/>
       <c r="J129" s="36"/>
     </row>

</xml_diff>

<commit_message>
added alternative term to 'prehospital training objective specification'
</commit_message>
<xml_diff>
--- a/TermSurveyResponses.xlsx
+++ b/TermSurveyResponses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathiasbrochhausen/OOSTT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED20E875-25AE-3643-A273-045BA58F1FB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004F45B6-0AEE-A54E-AC85-098215266892}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="460" windowWidth="27740" windowHeight="17540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="815">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="816">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -2512,6 +2512,9 @@
   </si>
   <si>
     <t>https://github.com/OOSTT/OOSTT/commit/977cd2ab7d9cbf50b74e74f7c46e7044bf9f6064 https://github.com/OOSTT/OOSTT/commit/a0dfe1a7e655bbdc1e1108766577e983b361fe5f https://github.com/OOSTT/OOSTT/commit/6b7bdceda63a4b599efcd2e97f4014377cdc0f17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To stay consistent with the genus differentia form, we will implement this suggestion. </t>
   </si>
 </sst>
 </file>
@@ -8892,8 +8895,8 @@
   <dimension ref="A1:IW1418"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J145" sqref="J145"/>
+      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H158" sqref="H158:H167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -11976,8 +11979,8 @@
       </c>
       <c r="E139" s="56"/>
       <c r="F139" s="37"/>
-      <c r="G139" s="60"/>
-      <c r="H139" s="36"/>
+      <c r="G139" s="36"/>
+      <c r="H139" s="60"/>
       <c r="I139" s="36"/>
       <c r="J139" s="36"/>
     </row>
@@ -11997,8 +12000,8 @@
       </c>
       <c r="E140" s="56"/>
       <c r="F140" s="37"/>
-      <c r="G140" s="60"/>
-      <c r="H140" s="36"/>
+      <c r="G140" s="36"/>
+      <c r="H140" s="60"/>
       <c r="I140" s="36"/>
       <c r="J140" s="36"/>
     </row>
@@ -12020,8 +12023,8 @@
       <c r="F141" s="57" t="s">
         <v>194</v>
       </c>
-      <c r="G141" s="60"/>
-      <c r="H141" s="36"/>
+      <c r="G141" s="36"/>
+      <c r="H141" s="60"/>
       <c r="I141" s="36"/>
       <c r="J141" s="36"/>
     </row>
@@ -12041,8 +12044,8 @@
       </c>
       <c r="E142" s="56"/>
       <c r="F142" s="37"/>
-      <c r="G142" s="60"/>
-      <c r="H142" s="36"/>
+      <c r="G142" s="36"/>
+      <c r="H142" s="60"/>
       <c r="I142" s="36"/>
       <c r="J142" s="36"/>
     </row>
@@ -12062,8 +12065,8 @@
       </c>
       <c r="E143" s="56"/>
       <c r="F143" s="37"/>
-      <c r="G143" s="60"/>
-      <c r="H143" s="36"/>
+      <c r="G143" s="36"/>
+      <c r="H143" s="60"/>
       <c r="I143" s="36"/>
       <c r="J143" s="36"/>
     </row>
@@ -12083,8 +12086,8 @@
       </c>
       <c r="E144" s="56"/>
       <c r="F144" s="37"/>
-      <c r="G144" s="60"/>
-      <c r="H144" s="36"/>
+      <c r="G144" s="36"/>
+      <c r="H144" s="60"/>
       <c r="I144" s="36"/>
       <c r="J144" s="36"/>
     </row>
@@ -12108,8 +12111,8 @@
       <c r="F145" s="57" t="s">
         <v>196</v>
       </c>
-      <c r="G145" s="60"/>
-      <c r="H145" s="36"/>
+      <c r="G145" s="36"/>
+      <c r="H145" s="60"/>
       <c r="I145" s="38" t="s">
         <v>813</v>
       </c>
@@ -12133,8 +12136,8 @@
       </c>
       <c r="E146" s="56"/>
       <c r="F146" s="37"/>
-      <c r="G146" s="60"/>
-      <c r="H146" s="36"/>
+      <c r="G146" s="36"/>
+      <c r="H146" s="60"/>
       <c r="I146" s="36"/>
       <c r="J146" s="36"/>
     </row>
@@ -12152,8 +12155,8 @@
       <c r="D147" s="58"/>
       <c r="E147" s="56"/>
       <c r="F147" s="37"/>
-      <c r="G147" s="60"/>
-      <c r="H147" s="36"/>
+      <c r="G147" s="36"/>
+      <c r="H147" s="60"/>
       <c r="I147" s="36"/>
       <c r="J147" s="36"/>
     </row>
@@ -12173,8 +12176,8 @@
       </c>
       <c r="E148" s="45"/>
       <c r="F148" s="46"/>
-      <c r="G148" s="47"/>
-      <c r="H148" s="47"/>
+      <c r="G148" s="36"/>
+      <c r="H148" s="60"/>
       <c r="I148" s="47"/>
       <c r="J148" s="47"/>
     </row>
@@ -12194,8 +12197,8 @@
       </c>
       <c r="E149" s="45"/>
       <c r="F149" s="46"/>
-      <c r="G149" s="47"/>
-      <c r="H149" s="47"/>
+      <c r="G149" s="36"/>
+      <c r="H149" s="60"/>
       <c r="I149" s="47"/>
       <c r="J149" s="47"/>
     </row>
@@ -12215,8 +12218,8 @@
       </c>
       <c r="E150" s="45"/>
       <c r="F150" s="46"/>
-      <c r="G150" s="47"/>
-      <c r="H150" s="47"/>
+      <c r="G150" s="36"/>
+      <c r="H150" s="60"/>
       <c r="I150" s="47"/>
       <c r="J150" s="47"/>
     </row>
@@ -12236,8 +12239,8 @@
       </c>
       <c r="E151" s="45"/>
       <c r="F151" s="46"/>
-      <c r="G151" s="47"/>
-      <c r="H151" s="47"/>
+      <c r="G151" s="36"/>
+      <c r="H151" s="60"/>
       <c r="I151" s="47"/>
       <c r="J151" s="47"/>
     </row>
@@ -12257,8 +12260,8 @@
       </c>
       <c r="E152" s="45"/>
       <c r="F152" s="46"/>
-      <c r="G152" s="47"/>
-      <c r="H152" s="47"/>
+      <c r="G152" s="36"/>
+      <c r="H152" s="60"/>
       <c r="I152" s="47"/>
       <c r="J152" s="47"/>
     </row>
@@ -12278,8 +12281,8 @@
       </c>
       <c r="E153" s="45"/>
       <c r="F153" s="46"/>
-      <c r="G153" s="47"/>
-      <c r="H153" s="47"/>
+      <c r="G153" s="36"/>
+      <c r="H153" s="60"/>
       <c r="I153" s="47"/>
       <c r="J153" s="47"/>
     </row>
@@ -12299,8 +12302,8 @@
       </c>
       <c r="E154" s="45"/>
       <c r="F154" s="46"/>
-      <c r="G154" s="47"/>
-      <c r="H154" s="47"/>
+      <c r="G154" s="36"/>
+      <c r="H154" s="60"/>
       <c r="I154" s="47"/>
       <c r="J154" s="47"/>
     </row>
@@ -12320,8 +12323,8 @@
       </c>
       <c r="E155" s="45"/>
       <c r="F155" s="46"/>
-      <c r="G155" s="47"/>
-      <c r="H155" s="47"/>
+      <c r="G155" s="36"/>
+      <c r="H155" s="60"/>
       <c r="I155" s="47"/>
       <c r="J155" s="47"/>
     </row>
@@ -12341,8 +12344,8 @@
       </c>
       <c r="E156" s="45"/>
       <c r="F156" s="46"/>
-      <c r="G156" s="47"/>
-      <c r="H156" s="47"/>
+      <c r="G156" s="36"/>
+      <c r="H156" s="60"/>
       <c r="I156" s="47"/>
       <c r="J156" s="47"/>
     </row>
@@ -12362,8 +12365,8 @@
       </c>
       <c r="E157" s="45"/>
       <c r="F157" s="46"/>
-      <c r="G157" s="47"/>
-      <c r="H157" s="47"/>
+      <c r="G157" s="36"/>
+      <c r="H157" s="60"/>
       <c r="I157" s="47"/>
       <c r="J157" s="47"/>
     </row>
@@ -12384,7 +12387,7 @@
       <c r="E158" s="56"/>
       <c r="F158" s="37"/>
       <c r="G158" s="36"/>
-      <c r="H158" s="36"/>
+      <c r="H158" s="60"/>
       <c r="I158" s="36"/>
       <c r="J158" s="36"/>
     </row>
@@ -12405,7 +12408,7 @@
       <c r="E159" s="56"/>
       <c r="F159" s="37"/>
       <c r="G159" s="36"/>
-      <c r="H159" s="36"/>
+      <c r="H159" s="60"/>
       <c r="I159" s="36"/>
       <c r="J159" s="36"/>
     </row>
@@ -12426,11 +12429,11 @@
       <c r="E160" s="56"/>
       <c r="F160" s="37"/>
       <c r="G160" s="36"/>
-      <c r="H160" s="36"/>
+      <c r="H160" s="60"/>
       <c r="I160" s="36"/>
       <c r="J160" s="36"/>
     </row>
-    <row r="161" spans="1:10" ht="14" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:10" ht="42" x14ac:dyDescent="0.15">
       <c r="A161" s="19">
         <v>23</v>
       </c>
@@ -12448,8 +12451,10 @@
         <v>197</v>
       </c>
       <c r="F161" s="37"/>
-      <c r="G161" s="36"/>
-      <c r="H161" s="36"/>
+      <c r="G161" s="38" t="s">
+        <v>815</v>
+      </c>
+      <c r="H161" s="60"/>
       <c r="I161" s="36"/>
       <c r="J161" s="36"/>
     </row>
@@ -12470,7 +12475,7 @@
       <c r="E162" s="56"/>
       <c r="F162" s="37"/>
       <c r="G162" s="36"/>
-      <c r="H162" s="36"/>
+      <c r="H162" s="60"/>
       <c r="I162" s="36"/>
       <c r="J162" s="36"/>
     </row>
@@ -12491,7 +12496,7 @@
       <c r="E163" s="56"/>
       <c r="F163" s="37"/>
       <c r="G163" s="36"/>
-      <c r="H163" s="36"/>
+      <c r="H163" s="60"/>
       <c r="I163" s="36"/>
       <c r="J163" s="36"/>
     </row>
@@ -12512,7 +12517,7 @@
       <c r="E164" s="56"/>
       <c r="F164" s="37"/>
       <c r="G164" s="36"/>
-      <c r="H164" s="36"/>
+      <c r="H164" s="60"/>
       <c r="I164" s="36"/>
       <c r="J164" s="36"/>
     </row>
@@ -12533,7 +12538,7 @@
       <c r="E165" s="56"/>
       <c r="F165" s="37"/>
       <c r="G165" s="36"/>
-      <c r="H165" s="36"/>
+      <c r="H165" s="60"/>
       <c r="I165" s="36"/>
       <c r="J165" s="36"/>
     </row>
@@ -12554,7 +12559,7 @@
       <c r="E166" s="56"/>
       <c r="F166" s="37"/>
       <c r="G166" s="36"/>
-      <c r="H166" s="36"/>
+      <c r="H166" s="60"/>
       <c r="I166" s="36"/>
       <c r="J166" s="36"/>
     </row>
@@ -12575,7 +12580,7 @@
       <c r="E167" s="56"/>
       <c r="F167" s="37"/>
       <c r="G167" s="36"/>
-      <c r="H167" s="36"/>
+      <c r="H167" s="60"/>
       <c r="I167" s="36"/>
       <c r="J167" s="36"/>
     </row>

</xml_diff>

<commit_message>
edited definition: TMD approved institution-specific emergency medicine physician profile
</commit_message>
<xml_diff>
--- a/TermSurveyResponses.xlsx
+++ b/TermSurveyResponses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathiasbrochhausen/OOSTT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA126DC-5824-9044-A098-7A9169EECC88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B23264-3073-E940-974C-48577E725B0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="460" windowWidth="27740" windowHeight="17540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="832">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="835">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -2563,6 +2563,15 @@
   </si>
   <si>
     <t>Based on the input of our expert team "protocls" aren't universally binding. Hence we will leave the definition and the term unalatered.</t>
+  </si>
+  <si>
+    <t>OOSTT user-centered definition: A professional organization focusing its mission on the improvement of trauma care within the region.</t>
+  </si>
+  <si>
+    <t>addressed as suggested.</t>
+  </si>
+  <si>
+    <t>https://github.com/OOSTT/OOSTT/commit/fba971795d296c2b2cb8bb6b3043e9d2334a9bfe</t>
   </si>
 </sst>
 </file>
@@ -8945,9 +8954,9 @@
   </sheetPr>
   <dimension ref="A1:IW1418"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H168" sqref="H168:H176"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J216" sqref="J216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -13578,7 +13587,7 @@
       <c r="E210" s="45"/>
       <c r="F210" s="46"/>
       <c r="G210" s="47"/>
-      <c r="H210" s="47"/>
+      <c r="H210" s="60"/>
       <c r="I210" s="47"/>
       <c r="J210" s="47"/>
     </row>
@@ -13599,7 +13608,7 @@
       <c r="E211" s="45"/>
       <c r="F211" s="46"/>
       <c r="G211" s="47"/>
-      <c r="H211" s="47"/>
+      <c r="H211" s="60"/>
       <c r="I211" s="47"/>
       <c r="J211" s="47"/>
     </row>
@@ -13620,7 +13629,7 @@
       <c r="E212" s="45"/>
       <c r="F212" s="46"/>
       <c r="G212" s="47"/>
-      <c r="H212" s="47"/>
+      <c r="H212" s="60"/>
       <c r="I212" s="47"/>
       <c r="J212" s="47"/>
     </row>
@@ -13641,7 +13650,7 @@
       <c r="E213" s="56"/>
       <c r="F213" s="37"/>
       <c r="G213" s="36"/>
-      <c r="H213" s="36"/>
+      <c r="H213" s="60"/>
       <c r="I213" s="36"/>
       <c r="J213" s="36"/>
     </row>
@@ -13662,7 +13671,7 @@
       <c r="E214" s="56"/>
       <c r="F214" s="37"/>
       <c r="G214" s="36"/>
-      <c r="H214" s="36"/>
+      <c r="H214" s="60"/>
       <c r="I214" s="36"/>
       <c r="J214" s="36"/>
     </row>
@@ -13683,11 +13692,11 @@
       <c r="E215" s="56"/>
       <c r="F215" s="37"/>
       <c r="G215" s="36"/>
-      <c r="H215" s="36"/>
+      <c r="H215" s="60"/>
       <c r="I215" s="36"/>
       <c r="J215" s="36"/>
     </row>
-    <row r="216" spans="1:10" ht="28" x14ac:dyDescent="0.15">
+    <row r="216" spans="1:10" ht="42" x14ac:dyDescent="0.15">
       <c r="A216" s="19">
         <v>36</v>
       </c>
@@ -13705,10 +13714,16 @@
       <c r="F216" s="57" t="s">
         <v>212</v>
       </c>
-      <c r="G216" s="36"/>
-      <c r="H216" s="36"/>
-      <c r="I216" s="36"/>
-      <c r="J216" s="36"/>
+      <c r="G216" s="36" t="s">
+        <v>833</v>
+      </c>
+      <c r="H216" s="60"/>
+      <c r="I216" s="38" t="s">
+        <v>832</v>
+      </c>
+      <c r="J216" s="38" t="s">
+        <v>834</v>
+      </c>
     </row>
     <row r="217" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A217" s="19">
@@ -13727,7 +13742,7 @@
       <c r="E217" s="56"/>
       <c r="F217" s="37"/>
       <c r="G217" s="36"/>
-      <c r="H217" s="36"/>
+      <c r="H217" s="60"/>
       <c r="I217" s="36"/>
       <c r="J217" s="36"/>
     </row>
@@ -13748,7 +13763,7 @@
       <c r="E218" s="56"/>
       <c r="F218" s="37"/>
       <c r="G218" s="36"/>
-      <c r="H218" s="36"/>
+      <c r="H218" s="60"/>
       <c r="I218" s="36"/>
       <c r="J218" s="36"/>
     </row>
@@ -13769,7 +13784,7 @@
       <c r="E219" s="56"/>
       <c r="F219" s="37"/>
       <c r="G219" s="36"/>
-      <c r="H219" s="36"/>
+      <c r="H219" s="60"/>
       <c r="I219" s="36"/>
       <c r="J219" s="36"/>
     </row>
@@ -13790,7 +13805,7 @@
       <c r="E220" s="56"/>
       <c r="F220" s="37"/>
       <c r="G220" s="36"/>
-      <c r="H220" s="36"/>
+      <c r="H220" s="60"/>
       <c r="I220" s="36"/>
       <c r="J220" s="36"/>
     </row>
@@ -13811,7 +13826,7 @@
       <c r="E221" s="56"/>
       <c r="F221" s="37"/>
       <c r="G221" s="36"/>
-      <c r="H221" s="36"/>
+      <c r="H221" s="60"/>
       <c r="I221" s="36"/>
       <c r="J221" s="36"/>
     </row>

</xml_diff>

<commit_message>
added comment: record of participation in majority of trauma peer review committee meetings
</commit_message>
<xml_diff>
--- a/TermSurveyResponses.xlsx
+++ b/TermSurveyResponses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathiasbrochhausen/OOSTT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AC83E1-8496-704E-8CD9-7211E91BC92F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE13B6DF-429E-394F-B442-9FBDB582C2EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10540" yWindow="460" windowWidth="27740" windowHeight="17540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9036,8 +9036,8 @@
   <dimension ref="A1:IW1418"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A269" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I273" sqref="I273"/>
+      <pane ySplit="1" topLeftCell="A267" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H268" sqref="H268:H277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -14950,7 +14950,7 @@
       <c r="E268" s="56"/>
       <c r="F268" s="37"/>
       <c r="G268" s="36"/>
-      <c r="H268" s="36"/>
+      <c r="H268" s="60"/>
       <c r="I268" s="36"/>
       <c r="J268" s="36"/>
     </row>
@@ -14971,7 +14971,7 @@
       <c r="E269" s="56"/>
       <c r="F269" s="37"/>
       <c r="G269" s="36"/>
-      <c r="H269" s="36"/>
+      <c r="H269" s="60"/>
       <c r="I269" s="36"/>
       <c r="J269" s="36"/>
     </row>
@@ -14992,7 +14992,7 @@
       <c r="E270" s="56"/>
       <c r="F270" s="37"/>
       <c r="G270" s="36"/>
-      <c r="H270" s="36"/>
+      <c r="H270" s="60"/>
       <c r="I270" s="36"/>
       <c r="J270" s="36"/>
     </row>
@@ -15017,7 +15017,7 @@
       <c r="G271" s="38" t="s">
         <v>851</v>
       </c>
-      <c r="H271" s="36"/>
+      <c r="H271" s="60"/>
       <c r="I271" s="36"/>
       <c r="J271" s="36"/>
     </row>
@@ -15042,7 +15042,7 @@
       <c r="G272" s="38" t="s">
         <v>850</v>
       </c>
-      <c r="H272" s="36"/>
+      <c r="H272" s="60"/>
       <c r="I272" s="36"/>
       <c r="J272" s="38" t="s">
         <v>853</v>
@@ -15069,7 +15069,7 @@
       <c r="G273" s="38" t="s">
         <v>852</v>
       </c>
-      <c r="H273" s="36"/>
+      <c r="H273" s="60"/>
       <c r="I273" s="38" t="s">
         <v>855</v>
       </c>
@@ -15094,7 +15094,7 @@
       <c r="E274" s="56"/>
       <c r="F274" s="37"/>
       <c r="G274" s="36"/>
-      <c r="H274" s="36"/>
+      <c r="H274" s="60"/>
       <c r="I274" s="36"/>
       <c r="J274" s="36"/>
     </row>
@@ -15115,7 +15115,7 @@
       <c r="E275" s="56"/>
       <c r="F275" s="37"/>
       <c r="G275" s="36"/>
-      <c r="H275" s="36"/>
+      <c r="H275" s="60"/>
       <c r="I275" s="36"/>
       <c r="J275" s="36"/>
     </row>
@@ -15136,7 +15136,7 @@
       <c r="E276" s="56"/>
       <c r="F276" s="37"/>
       <c r="G276" s="36"/>
-      <c r="H276" s="36"/>
+      <c r="H276" s="60"/>
       <c r="I276" s="36"/>
       <c r="J276" s="36"/>
     </row>
@@ -15157,7 +15157,7 @@
       <c r="E277" s="56"/>
       <c r="F277" s="37"/>
       <c r="G277" s="36"/>
-      <c r="H277" s="36"/>
+      <c r="H277" s="60"/>
       <c r="I277" s="36"/>
       <c r="J277" s="36"/>
     </row>

</xml_diff>

<commit_message>
Spreadsheet with documented changes
</commit_message>
<xml_diff>
--- a/TermSurveyResponses.xlsx
+++ b/TermSurveyResponses.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="1041">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="1047">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -2888,9 +2888,6 @@
     <t xml:space="preserve">Accept "anesthesiology credentialed members" change. Resolves issues raised by respondent 300. </t>
   </si>
   <si>
-    <t>Accept but strike "multi-specialty."</t>
-  </si>
-  <si>
     <t>Reject. Why delete it?</t>
   </si>
   <si>
@@ -2957,9 +2954,6 @@
     <t>Below should correct problem</t>
   </si>
   <si>
-    <t>Not sure what respondent means by "authoritative organizations."</t>
-  </si>
-  <si>
     <t xml:space="preserve">Reject; I don't think the term is meant to define the process. </t>
   </si>
   <si>
@@ -3099,9 +3093,6 @@
   </si>
   <si>
     <t xml:space="preserve">Ignore; no suggestion for how to improve definition </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ask Mathias: should we providemore description of the expectation? </t>
   </si>
   <si>
     <t>Sarah's new definition</t>
@@ -3207,6 +3198,33 @@
   </si>
   <si>
     <t>Reject; don't think this is true</t>
+  </si>
+  <si>
+    <t>A healthcare facility policy that specifies the requirement for anesthesiology-credentialed members availability 24 hours a day, 7 days a week.</t>
+  </si>
+  <si>
+    <t>An organized and regulated local, state, provincial, regional, or national approach to facilitating and coordinating a multidisciplinary medical system response to severely injured patients.</t>
+  </si>
+  <si>
+    <t>A Level I trauma center role is borne by a hospital that provides the highest level of surgical care to trauma patients. Its bearer has a full range of specialists and equipment available 24 hours a day and admits a minimum required annual volume of severely injured patients established by the verifying agency. The facility has transfer agreements with referring facilities, and provides performance improvement and education outreach to those facilities. The facility also has an ongoing program of research and a physician residency program. The role is created by a Level I Trauma Center designation.</t>
+  </si>
+  <si>
+    <t>A state, regional, provincial, or national recognition process in which a facility is awarded a trauma center role after a formal review of the hospital's organization, capacity, personnel, and resources by a verifying agency.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ask Mathias: should we provide more description of the expectation? </t>
+  </si>
+  <si>
+    <t>A trauma center role that is borne by a hospital that is organized to provide trauma care to injured infants, children, and adolescents.  Its bearer has a full range of pediatric specialists and equipment available 24 hours a day and admits a minimum required annual volume of severely injured patients established by the designating agency. The facility has transfer agreements with referring facilities, and provides performance improvement and education outreach to those facilities. The role is created by a pediatric Trauma Center designation.</t>
+  </si>
+  <si>
+    <t>The description of content and expected learning for health professionals that is necessary to maintain continued competency and to learn new and developing concepts in medical care.</t>
+  </si>
+  <si>
+    <t>The entity with the power to develop, oversee, improve medical care, and implement corrective actions following a performance improvement process for injured patients in the healthcare facility.</t>
+  </si>
+  <si>
+    <t>A medical residency in anesthesiology required for board certification as an anesthesiologist.</t>
   </si>
 </sst>
 </file>
@@ -9682,8 +9700,8 @@
   <dimension ref="A1:IW1418"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A813" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K826" sqref="K826"/>
+      <pane ySplit="1" topLeftCell="A991" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K1000" sqref="K1000"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.33203125" defaultRowHeight="19.95" customHeight="1"/>
@@ -9739,10 +9757,10 @@
         <v>864</v>
       </c>
       <c r="L1" s="69" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
       <c r="M1" s="69" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="N1" s="29" t="s">
         <v>775</v>
@@ -16113,7 +16131,7 @@
         <v>867</v>
       </c>
       <c r="L289" s="82" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="M289" s="82" t="s">
         <v>548</v>
@@ -16279,10 +16297,10 @@
         <v>894</v>
       </c>
       <c r="L296" s="82" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="M296" s="82" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="297" spans="1:13" ht="66">
@@ -16661,7 +16679,7 @@
         <v>869</v>
       </c>
       <c r="L313" s="82" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
       <c r="M313" s="82" t="s">
         <v>552</v>
@@ -17065,7 +17083,7 @@
       <c r="I332" s="46"/>
       <c r="J332" s="73"/>
       <c r="K332" s="83" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="333" spans="1:11" ht="13.2">
@@ -17276,7 +17294,7 @@
         <v>871</v>
       </c>
       <c r="L341" s="82" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="M341" s="82" t="s">
         <v>560</v>
@@ -18139,7 +18157,7 @@
       <c r="I381" s="36"/>
       <c r="J381" s="71"/>
       <c r="K381" s="83" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="382" spans="1:11" ht="26.4">
@@ -18399,7 +18417,7 @@
       <c r="I393" s="46"/>
       <c r="J393" s="73"/>
       <c r="K393" s="83" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="394" spans="1:11" ht="26.4">
@@ -19129,10 +19147,10 @@
         <v>880</v>
       </c>
       <c r="L427" s="82" t="s">
-        <v>1023</v>
+        <v>1020</v>
       </c>
       <c r="M427" s="82" t="s">
-        <v>1022</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="428" spans="1:13" ht="13.2">
@@ -19582,7 +19600,7 @@
         <v>882</v>
       </c>
       <c r="L448" s="82" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
       <c r="M448" s="82" t="s">
         <v>581</v>
@@ -20057,7 +20075,7 @@
         <v>886</v>
       </c>
       <c r="L469" s="82" t="s">
-        <v>1025</v>
+        <v>1022</v>
       </c>
       <c r="M469" s="82" t="s">
         <v>585</v>
@@ -20405,7 +20423,7 @@
       <c r="I485" s="36"/>
       <c r="J485" s="71"/>
       <c r="K485" s="82" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="486" spans="1:13" ht="26.4">
@@ -20567,7 +20585,7 @@
         <v>890</v>
       </c>
       <c r="L492" s="82" t="s">
-        <v>1027</v>
+        <v>1024</v>
       </c>
       <c r="M492" s="82" t="s">
         <v>591</v>
@@ -21560,7 +21578,7 @@
         <v>896</v>
       </c>
       <c r="L538" s="82" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
       <c r="M538" s="82" t="s">
         <v>601</v>
@@ -22386,7 +22404,7 @@
         <v>904</v>
       </c>
       <c r="L575" s="82" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
       <c r="M575" s="82" t="s">
         <v>609</v>
@@ -22962,7 +22980,7 @@
       <c r="I602" s="46"/>
       <c r="J602" s="73"/>
       <c r="K602" s="83" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="603" spans="1:11" ht="13.2">
@@ -23161,7 +23179,7 @@
       <c r="I611" s="36"/>
       <c r="J611" s="71"/>
       <c r="K611" s="83" t="s">
-        <v>1031</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="612" spans="1:11" ht="26.4">
@@ -24338,7 +24356,7 @@
         <v>922</v>
       </c>
       <c r="L664" s="82" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="M664" s="82" t="s">
         <v>629</v>
@@ -24576,7 +24594,7 @@
       <c r="I674" s="46"/>
       <c r="J674" s="73"/>
       <c r="K674" s="82" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="675" spans="1:13" ht="13.2">
@@ -24689,7 +24707,7 @@
         <v>924</v>
       </c>
       <c r="L679" s="82" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="M679" s="82" t="s">
         <v>631</v>
@@ -25299,7 +25317,7 @@
         <v>926</v>
       </c>
       <c r="L707" s="82" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
       <c r="M707" s="82" t="s">
         <v>637</v>
@@ -26289,7 +26307,7 @@
         <v>928</v>
       </c>
       <c r="L752" s="82" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="M752" s="82" t="s">
         <v>647</v>
@@ -26410,7 +26428,7 @@
         <v>932</v>
       </c>
       <c r="L757" s="82" t="s">
-        <v>1039</v>
+        <v>1036</v>
       </c>
       <c r="M757" s="82" t="s">
         <v>649</v>
@@ -27700,7 +27718,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="817" spans="1:11" ht="26.4">
+    <row r="817" spans="1:13" ht="26.4">
       <c r="A817" s="19">
         <v>136</v>
       </c>
@@ -27721,7 +27739,7 @@
       <c r="I817" s="36"/>
       <c r="J817" s="71"/>
     </row>
-    <row r="818" spans="1:11" ht="13.2">
+    <row r="818" spans="1:13" ht="13.2">
       <c r="A818" s="19">
         <v>137</v>
       </c>
@@ -27742,7 +27760,7 @@
       <c r="I818" s="46"/>
       <c r="J818" s="73"/>
     </row>
-    <row r="819" spans="1:11" ht="13.2">
+    <row r="819" spans="1:13" ht="13.2">
       <c r="A819" s="19">
         <v>137</v>
       </c>
@@ -27763,7 +27781,7 @@
       <c r="I819" s="46"/>
       <c r="J819" s="73"/>
     </row>
-    <row r="820" spans="1:11" ht="13.2">
+    <row r="820" spans="1:13" ht="13.2">
       <c r="A820" s="19">
         <v>137</v>
       </c>
@@ -27784,7 +27802,7 @@
       <c r="I820" s="46"/>
       <c r="J820" s="73"/>
     </row>
-    <row r="821" spans="1:11" ht="52.8">
+    <row r="821" spans="1:13" ht="79.2">
       <c r="A821" s="19">
         <v>137</v>
       </c>
@@ -27811,8 +27829,14 @@
       <c r="K821" s="82" t="s">
         <v>939</v>
       </c>
-    </row>
-    <row r="822" spans="1:11" ht="13.2">
+      <c r="L821" s="82" t="s">
+        <v>1038</v>
+      </c>
+      <c r="M821" s="82" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="822" spans="1:13" ht="13.2">
       <c r="A822" s="19">
         <v>137</v>
       </c>
@@ -27833,7 +27857,7 @@
       <c r="I822" s="46"/>
       <c r="J822" s="73"/>
     </row>
-    <row r="823" spans="1:11" ht="39.6">
+    <row r="823" spans="1:13" ht="39.6">
       <c r="A823" s="19">
         <v>137</v>
       </c>
@@ -27858,10 +27882,10 @@
       <c r="I823" s="46"/>
       <c r="J823" s="73"/>
       <c r="K823" s="83" t="s">
-        <v>1040</v>
-      </c>
-    </row>
-    <row r="824" spans="1:11" ht="13.2">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="824" spans="1:13" ht="13.2">
       <c r="A824" s="19">
         <v>137</v>
       </c>
@@ -27882,7 +27906,7 @@
       <c r="I824" s="46"/>
       <c r="J824" s="73"/>
     </row>
-    <row r="825" spans="1:11" ht="13.2">
+    <row r="825" spans="1:13" ht="13.2">
       <c r="A825" s="19">
         <v>137</v>
       </c>
@@ -27903,7 +27927,7 @@
       <c r="I825" s="46"/>
       <c r="J825" s="73"/>
     </row>
-    <row r="826" spans="1:11" ht="27.6">
+    <row r="826" spans="1:13" ht="27.6">
       <c r="A826" s="19">
         <v>137</v>
       </c>
@@ -27929,7 +27953,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="827" spans="1:11" ht="13.2">
+    <row r="827" spans="1:13" ht="13.2">
       <c r="A827" s="19">
         <v>138</v>
       </c>
@@ -27948,7 +27972,7 @@
       <c r="I827" s="36"/>
       <c r="J827" s="71"/>
     </row>
-    <row r="828" spans="1:11" ht="13.2">
+    <row r="828" spans="1:13" ht="13.2">
       <c r="A828" s="19">
         <v>138</v>
       </c>
@@ -27969,7 +27993,7 @@
       <c r="I828" s="36"/>
       <c r="J828" s="71"/>
     </row>
-    <row r="829" spans="1:11" ht="13.2">
+    <row r="829" spans="1:13" ht="13.2">
       <c r="A829" s="19">
         <v>138</v>
       </c>
@@ -27990,7 +28014,7 @@
       <c r="I829" s="36"/>
       <c r="J829" s="71"/>
     </row>
-    <row r="830" spans="1:11" ht="13.2">
+    <row r="830" spans="1:13" ht="13.2">
       <c r="A830" s="19">
         <v>138</v>
       </c>
@@ -28009,7 +28033,7 @@
       <c r="I830" s="36"/>
       <c r="J830" s="71"/>
     </row>
-    <row r="831" spans="1:11" ht="13.2">
+    <row r="831" spans="1:13" ht="13.2">
       <c r="A831" s="19">
         <v>138</v>
       </c>
@@ -28030,7 +28054,7 @@
       <c r="I831" s="36"/>
       <c r="J831" s="71"/>
     </row>
-    <row r="832" spans="1:11" ht="13.2">
+    <row r="832" spans="1:13" ht="13.2">
       <c r="A832" s="19">
         <v>138</v>
       </c>
@@ -28051,7 +28075,7 @@
       <c r="I832" s="36"/>
       <c r="J832" s="71"/>
     </row>
-    <row r="833" spans="1:11" ht="13.2">
+    <row r="833" spans="1:13" ht="13.2">
       <c r="A833" s="19">
         <v>138</v>
       </c>
@@ -28072,7 +28096,7 @@
       <c r="I833" s="36"/>
       <c r="J833" s="71"/>
     </row>
-    <row r="834" spans="1:11" ht="13.2">
+    <row r="834" spans="1:13" ht="13.2">
       <c r="A834" s="19">
         <v>138</v>
       </c>
@@ -28093,7 +28117,7 @@
       <c r="I834" s="36"/>
       <c r="J834" s="71"/>
     </row>
-    <row r="835" spans="1:11" ht="13.2">
+    <row r="835" spans="1:13" ht="13.2">
       <c r="A835" s="19">
         <v>138</v>
       </c>
@@ -28114,7 +28138,7 @@
       <c r="I835" s="36"/>
       <c r="J835" s="71"/>
     </row>
-    <row r="836" spans="1:11" ht="13.2">
+    <row r="836" spans="1:13" ht="13.2">
       <c r="A836" s="19">
         <v>140</v>
       </c>
@@ -28135,7 +28159,7 @@
       <c r="I836" s="46"/>
       <c r="J836" s="73"/>
     </row>
-    <row r="837" spans="1:11" ht="13.2">
+    <row r="837" spans="1:13" ht="13.2">
       <c r="A837" s="19">
         <v>140</v>
       </c>
@@ -28156,7 +28180,7 @@
       <c r="I837" s="46"/>
       <c r="J837" s="73"/>
     </row>
-    <row r="838" spans="1:11" ht="79.2">
+    <row r="838" spans="1:13" ht="79.2">
       <c r="A838" s="19">
         <v>140</v>
       </c>
@@ -28179,10 +28203,10 @@
       <c r="I838" s="46"/>
       <c r="J838" s="73"/>
       <c r="K838" s="82" t="s">
-        <v>940</v>
-      </c>
-    </row>
-    <row r="839" spans="1:11" ht="13.2">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="839" spans="1:13" ht="13.2">
       <c r="A839" s="19">
         <v>140</v>
       </c>
@@ -28203,7 +28227,7 @@
       <c r="I839" s="46"/>
       <c r="J839" s="73"/>
     </row>
-    <row r="840" spans="1:11" ht="13.2">
+    <row r="840" spans="1:13" ht="13.2">
       <c r="A840" s="19">
         <v>140</v>
       </c>
@@ -28224,7 +28248,7 @@
       <c r="I840" s="46"/>
       <c r="J840" s="73"/>
     </row>
-    <row r="841" spans="1:11" ht="13.2">
+    <row r="841" spans="1:13" ht="13.2">
       <c r="A841" s="19">
         <v>140</v>
       </c>
@@ -28245,7 +28269,7 @@
       <c r="I841" s="46"/>
       <c r="J841" s="73"/>
     </row>
-    <row r="842" spans="1:11" ht="13.2">
+    <row r="842" spans="1:13" ht="13.2">
       <c r="A842" s="19">
         <v>140</v>
       </c>
@@ -28266,7 +28290,7 @@
       <c r="I842" s="46"/>
       <c r="J842" s="73"/>
     </row>
-    <row r="843" spans="1:11" ht="13.2">
+    <row r="843" spans="1:13" ht="13.2">
       <c r="A843" s="19">
         <v>140</v>
       </c>
@@ -28287,7 +28311,7 @@
       <c r="I843" s="46"/>
       <c r="J843" s="73"/>
     </row>
-    <row r="844" spans="1:11" ht="13.2">
+    <row r="844" spans="1:13" ht="13.2">
       <c r="A844" s="19">
         <v>140</v>
       </c>
@@ -28308,7 +28332,7 @@
       <c r="I844" s="46"/>
       <c r="J844" s="73"/>
     </row>
-    <row r="845" spans="1:11" ht="13.2">
+    <row r="845" spans="1:13" ht="13.2">
       <c r="A845" s="19">
         <v>141</v>
       </c>
@@ -28331,10 +28355,10 @@
       <c r="I845" s="36"/>
       <c r="J845" s="71"/>
       <c r="K845" s="82" t="s">
-        <v>941</v>
-      </c>
-    </row>
-    <row r="846" spans="1:11" ht="13.2">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="846" spans="1:13" ht="13.2">
       <c r="A846" s="19">
         <v>141</v>
       </c>
@@ -28355,7 +28379,7 @@
       <c r="I846" s="36"/>
       <c r="J846" s="71"/>
     </row>
-    <row r="847" spans="1:11" ht="13.2">
+    <row r="847" spans="1:13" ht="13.2">
       <c r="A847" s="19">
         <v>141</v>
       </c>
@@ -28374,7 +28398,7 @@
       <c r="I847" s="36"/>
       <c r="J847" s="71"/>
     </row>
-    <row r="848" spans="1:11" ht="13.2">
+    <row r="848" spans="1:13" ht="105.6">
       <c r="A848" s="19">
         <v>141</v>
       </c>
@@ -28399,8 +28423,14 @@
       <c r="K848" s="82" t="s">
         <v>929</v>
       </c>
-    </row>
-    <row r="849" spans="1:11" ht="13.2">
+      <c r="L848" s="82" t="s">
+        <v>1039</v>
+      </c>
+      <c r="M848" s="82" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="849" spans="1:13" ht="13.2">
       <c r="A849" s="19">
         <v>141</v>
       </c>
@@ -28421,7 +28451,7 @@
       <c r="I849" s="36"/>
       <c r="J849" s="71"/>
     </row>
-    <row r="850" spans="1:11" ht="13.2">
+    <row r="850" spans="1:13" ht="13.2">
       <c r="A850" s="19">
         <v>141</v>
       </c>
@@ -28442,7 +28472,7 @@
       <c r="I850" s="36"/>
       <c r="J850" s="71"/>
     </row>
-    <row r="851" spans="1:11" ht="13.2">
+    <row r="851" spans="1:13" ht="13.2">
       <c r="A851" s="19">
         <v>141</v>
       </c>
@@ -28463,7 +28493,7 @@
       <c r="I851" s="36"/>
       <c r="J851" s="71"/>
     </row>
-    <row r="852" spans="1:11" ht="13.2">
+    <row r="852" spans="1:13" ht="13.2">
       <c r="A852" s="19">
         <v>141</v>
       </c>
@@ -28489,7 +28519,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="853" spans="1:11" ht="105.6">
+    <row r="853" spans="1:13" ht="124.2">
       <c r="A853" s="19">
         <v>141</v>
       </c>
@@ -28511,11 +28541,11 @@
       <c r="H853" s="36"/>
       <c r="I853" s="36"/>
       <c r="J853" s="71"/>
-      <c r="K853" s="82" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="854" spans="1:11" ht="13.2">
+      <c r="K853" s="83" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="854" spans="1:13" ht="13.2">
       <c r="A854" s="19">
         <v>142</v>
       </c>
@@ -28534,7 +28564,7 @@
       <c r="I854" s="46"/>
       <c r="J854" s="73"/>
     </row>
-    <row r="855" spans="1:11" ht="13.2">
+    <row r="855" spans="1:13" ht="13.2">
       <c r="A855" s="19">
         <v>142</v>
       </c>
@@ -28555,7 +28585,7 @@
       <c r="I855" s="46"/>
       <c r="J855" s="73"/>
     </row>
-    <row r="856" spans="1:11" ht="52.8">
+    <row r="856" spans="1:13" ht="52.8">
       <c r="A856" s="19">
         <v>142</v>
       </c>
@@ -28578,10 +28608,10 @@
       <c r="I856" s="46"/>
       <c r="J856" s="73"/>
       <c r="K856" s="82" t="s">
-        <v>942</v>
-      </c>
-    </row>
-    <row r="857" spans="1:11" ht="250.8">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="857" spans="1:13" ht="330">
       <c r="A857" s="19">
         <v>142</v>
       </c>
@@ -28604,10 +28634,16 @@
       <c r="I857" s="46"/>
       <c r="J857" s="73"/>
       <c r="K857" s="82" t="s">
-        <v>944</v>
-      </c>
-    </row>
-    <row r="858" spans="1:11" ht="79.2">
+        <v>943</v>
+      </c>
+      <c r="L857" s="82" t="s">
+        <v>1040</v>
+      </c>
+      <c r="M857" s="82" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="858" spans="1:13" ht="79.2">
       <c r="A858" s="19">
         <v>142</v>
       </c>
@@ -28627,11 +28663,11 @@
       <c r="H858" s="46"/>
       <c r="I858" s="46"/>
       <c r="J858" s="73"/>
-      <c r="K858" s="82" t="s">
-        <v>943</v>
-      </c>
-    </row>
-    <row r="859" spans="1:11" ht="13.2">
+      <c r="K858" s="83" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="859" spans="1:13" ht="13.2">
       <c r="A859" s="19">
         <v>142</v>
       </c>
@@ -28652,7 +28688,7 @@
       <c r="I859" s="46"/>
       <c r="J859" s="73"/>
     </row>
-    <row r="860" spans="1:11" ht="13.2">
+    <row r="860" spans="1:13" ht="13.2">
       <c r="A860" s="19">
         <v>142</v>
       </c>
@@ -28673,7 +28709,7 @@
       <c r="I860" s="46"/>
       <c r="J860" s="73"/>
     </row>
-    <row r="861" spans="1:11" ht="237.6">
+    <row r="861" spans="1:13" ht="237.6">
       <c r="A861" s="19">
         <v>142</v>
       </c>
@@ -28696,10 +28732,10 @@
       <c r="I861" s="46"/>
       <c r="J861" s="73"/>
       <c r="K861" s="82" t="s">
-        <v>946</v>
-      </c>
-    </row>
-    <row r="862" spans="1:11" ht="79.2">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="862" spans="1:13" ht="79.2">
       <c r="A862" s="19">
         <v>142</v>
       </c>
@@ -28722,10 +28758,10 @@
       <c r="I862" s="46"/>
       <c r="J862" s="73"/>
       <c r="K862" s="82" t="s">
-        <v>947</v>
-      </c>
-    </row>
-    <row r="863" spans="1:11" ht="13.2">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="863" spans="1:13" ht="13.2">
       <c r="A863" s="19">
         <v>145</v>
       </c>
@@ -28746,7 +28782,7 @@
       <c r="I863" s="36"/>
       <c r="J863" s="71"/>
     </row>
-    <row r="864" spans="1:11" ht="13.2">
+    <row r="864" spans="1:13" ht="13.2">
       <c r="A864" s="19">
         <v>145</v>
       </c>
@@ -28935,7 +28971,7 @@
       <c r="I872" s="46"/>
       <c r="J872" s="73"/>
       <c r="K872" s="82" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="873" spans="1:11" ht="13.2">
@@ -29096,7 +29132,7 @@
       <c r="I879" s="46"/>
       <c r="J879" s="73"/>
       <c r="K879" s="82" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="880" spans="1:11" ht="13.2">
@@ -29120,7 +29156,7 @@
       <c r="I880" s="46"/>
       <c r="J880" s="73"/>
     </row>
-    <row r="881" spans="1:11" ht="13.2">
+    <row r="881" spans="1:13" ht="13.2">
       <c r="A881" s="19">
         <v>147</v>
       </c>
@@ -29141,7 +29177,7 @@
       <c r="I881" s="46"/>
       <c r="J881" s="73"/>
     </row>
-    <row r="882" spans="1:11" ht="13.2">
+    <row r="882" spans="1:13" ht="13.2">
       <c r="A882" s="19">
         <v>147</v>
       </c>
@@ -29162,7 +29198,7 @@
       <c r="I882" s="46"/>
       <c r="J882" s="73"/>
     </row>
-    <row r="883" spans="1:11" ht="13.2">
+    <row r="883" spans="1:13" ht="13.2">
       <c r="A883" s="19">
         <v>147</v>
       </c>
@@ -29183,7 +29219,7 @@
       <c r="I883" s="46"/>
       <c r="J883" s="73"/>
     </row>
-    <row r="884" spans="1:11" ht="13.2">
+    <row r="884" spans="1:13" ht="13.2">
       <c r="A884" s="19">
         <v>147</v>
       </c>
@@ -29209,7 +29245,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="885" spans="1:11" ht="26.4">
+    <row r="885" spans="1:13" ht="26.4">
       <c r="A885" s="19">
         <v>147</v>
       </c>
@@ -29230,7 +29266,7 @@
       <c r="I885" s="46"/>
       <c r="J885" s="73"/>
     </row>
-    <row r="886" spans="1:11" ht="13.2">
+    <row r="886" spans="1:13" ht="13.2">
       <c r="A886" s="19">
         <v>147</v>
       </c>
@@ -29251,7 +29287,7 @@
       <c r="I886" s="46"/>
       <c r="J886" s="73"/>
     </row>
-    <row r="887" spans="1:11" ht="13.2">
+    <row r="887" spans="1:13" ht="13.2">
       <c r="A887" s="19">
         <v>147</v>
       </c>
@@ -29272,7 +29308,7 @@
       <c r="I887" s="46"/>
       <c r="J887" s="73"/>
     </row>
-    <row r="888" spans="1:11" ht="13.2">
+    <row r="888" spans="1:13" ht="13.2">
       <c r="A888" s="19">
         <v>147</v>
       </c>
@@ -29293,7 +29329,7 @@
       <c r="I888" s="46"/>
       <c r="J888" s="73"/>
     </row>
-    <row r="889" spans="1:11" ht="13.2">
+    <row r="889" spans="1:13" ht="13.2">
       <c r="A889" s="19">
         <v>147</v>
       </c>
@@ -29314,7 +29350,7 @@
       <c r="I889" s="46"/>
       <c r="J889" s="73"/>
     </row>
-    <row r="890" spans="1:11" ht="145.19999999999999">
+    <row r="890" spans="1:13" ht="145.19999999999999">
       <c r="A890" s="19">
         <v>147</v>
       </c>
@@ -29335,10 +29371,16 @@
       <c r="I890" s="46"/>
       <c r="J890" s="73"/>
       <c r="K890" s="82" t="s">
-        <v>949</v>
-      </c>
-    </row>
-    <row r="891" spans="1:11" ht="13.2">
+        <v>948</v>
+      </c>
+      <c r="L890" s="82" t="s">
+        <v>1041</v>
+      </c>
+      <c r="M890" s="82" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="891" spans="1:13" ht="13.2">
       <c r="A891" s="19">
         <v>148</v>
       </c>
@@ -29364,7 +29406,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="892" spans="1:11" ht="13.2">
+    <row r="892" spans="1:13" ht="13.2">
       <c r="A892" s="19">
         <v>148</v>
       </c>
@@ -29385,7 +29427,7 @@
       <c r="I892" s="36"/>
       <c r="J892" s="71"/>
     </row>
-    <row r="893" spans="1:11" ht="13.2">
+    <row r="893" spans="1:13" ht="13.2">
       <c r="A893" s="19">
         <v>148</v>
       </c>
@@ -29404,7 +29446,7 @@
       <c r="I893" s="36"/>
       <c r="J893" s="71"/>
     </row>
-    <row r="894" spans="1:11" ht="39.6">
+    <row r="894" spans="1:13" ht="330">
       <c r="A894" s="19">
         <v>148</v>
       </c>
@@ -29427,10 +29469,16 @@
       <c r="I894" s="36"/>
       <c r="J894" s="71"/>
       <c r="K894" s="82" t="s">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="895" spans="1:11" ht="13.2">
+        <v>950</v>
+      </c>
+      <c r="L894" s="82" t="s">
+        <v>1043</v>
+      </c>
+      <c r="M894" s="82" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="895" spans="1:13" ht="13.2">
       <c r="A895" s="19">
         <v>148</v>
       </c>
@@ -29451,7 +29499,7 @@
       <c r="I895" s="36"/>
       <c r="J895" s="71"/>
     </row>
-    <row r="896" spans="1:11" ht="13.2">
+    <row r="896" spans="1:13" ht="13.2">
       <c r="A896" s="19">
         <v>148</v>
       </c>
@@ -29641,8 +29689,8 @@
       <c r="H904" s="46"/>
       <c r="I904" s="46"/>
       <c r="J904" s="73"/>
-      <c r="K904" s="82" t="s">
-        <v>952</v>
+      <c r="K904" s="83" t="s">
+        <v>951</v>
       </c>
     </row>
     <row r="905" spans="1:11" ht="13.2">
@@ -29710,7 +29758,7 @@
       <c r="I907" s="46"/>
       <c r="J907" s="73"/>
       <c r="K907" s="82" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="908" spans="1:11" ht="13.2">
@@ -30041,8 +30089,8 @@
       <c r="H922" s="46"/>
       <c r="I922" s="46"/>
       <c r="J922" s="73"/>
-      <c r="K922" s="82" t="s">
-        <v>954</v>
+      <c r="K922" s="83" t="s">
+        <v>953</v>
       </c>
     </row>
     <row r="923" spans="1:11" ht="13.2">
@@ -30276,7 +30324,7 @@
       <c r="I933" s="36"/>
       <c r="J933" s="71"/>
       <c r="K933" s="83" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="934" spans="1:13" ht="13.2">
@@ -30347,10 +30395,10 @@
       <c r="I936" s="36"/>
       <c r="J936" s="71"/>
       <c r="K936" s="82" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="L936" s="82" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="M936" s="82" t="s">
         <v>686</v>
@@ -30444,7 +30492,7 @@
       <c r="I940" s="46"/>
       <c r="J940" s="73"/>
       <c r="K940" s="82" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="941" spans="1:13" ht="26.4">
@@ -30512,7 +30560,7 @@
       <c r="I943" s="46"/>
       <c r="J943" s="73"/>
       <c r="K943" s="82" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="944" spans="1:13" ht="26.4">
@@ -30536,7 +30584,7 @@
       <c r="I944" s="46"/>
       <c r="J944" s="73"/>
     </row>
-    <row r="945" spans="1:11" ht="26.4">
+    <row r="945" spans="1:13" ht="92.4">
       <c r="A945" s="19">
         <v>153</v>
       </c>
@@ -30557,10 +30605,16 @@
       <c r="I945" s="46"/>
       <c r="J945" s="73"/>
       <c r="K945" s="82" t="s">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="946" spans="1:11" ht="26.4">
+        <v>958</v>
+      </c>
+      <c r="L945" s="82" t="s">
+        <v>1044</v>
+      </c>
+      <c r="M945" s="82" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="946" spans="1:13" ht="26.4">
       <c r="A946" s="19">
         <v>154</v>
       </c>
@@ -30579,7 +30633,7 @@
       <c r="I946" s="36"/>
       <c r="J946" s="71"/>
     </row>
-    <row r="947" spans="1:11" ht="26.4">
+    <row r="947" spans="1:13" ht="26.4">
       <c r="A947" s="19">
         <v>154</v>
       </c>
@@ -30600,7 +30654,7 @@
       <c r="I947" s="36"/>
       <c r="J947" s="71"/>
     </row>
-    <row r="948" spans="1:11" ht="26.4">
+    <row r="948" spans="1:13" ht="26.4">
       <c r="A948" s="19">
         <v>154</v>
       </c>
@@ -30621,7 +30675,7 @@
       <c r="I948" s="36"/>
       <c r="J948" s="71"/>
     </row>
-    <row r="949" spans="1:11" ht="26.4">
+    <row r="949" spans="1:13" ht="26.4">
       <c r="A949" s="19">
         <v>154</v>
       </c>
@@ -30642,7 +30696,7 @@
       <c r="I949" s="36"/>
       <c r="J949" s="71"/>
     </row>
-    <row r="950" spans="1:11" ht="26.4">
+    <row r="950" spans="1:13" ht="26.4">
       <c r="A950" s="19">
         <v>154</v>
       </c>
@@ -30663,7 +30717,7 @@
       <c r="I950" s="36"/>
       <c r="J950" s="71"/>
     </row>
-    <row r="951" spans="1:11" ht="26.4">
+    <row r="951" spans="1:13" ht="26.4">
       <c r="A951" s="19">
         <v>154</v>
       </c>
@@ -30684,7 +30738,7 @@
       <c r="I951" s="36"/>
       <c r="J951" s="71"/>
     </row>
-    <row r="952" spans="1:11" ht="26.4">
+    <row r="952" spans="1:13" ht="26.4">
       <c r="A952" s="19">
         <v>154</v>
       </c>
@@ -30705,7 +30759,7 @@
       <c r="I952" s="36"/>
       <c r="J952" s="71"/>
     </row>
-    <row r="953" spans="1:11" ht="26.4">
+    <row r="953" spans="1:13" ht="26.4">
       <c r="A953" s="19">
         <v>154</v>
       </c>
@@ -30726,7 +30780,7 @@
       <c r="I953" s="36"/>
       <c r="J953" s="71"/>
     </row>
-    <row r="954" spans="1:11" ht="26.4">
+    <row r="954" spans="1:13" ht="26.4">
       <c r="A954" s="19">
         <v>154</v>
       </c>
@@ -30747,7 +30801,7 @@
       <c r="I954" s="36"/>
       <c r="J954" s="71"/>
     </row>
-    <row r="955" spans="1:11" ht="13.2">
+    <row r="955" spans="1:13" ht="13.2">
       <c r="A955" s="19">
         <v>155</v>
       </c>
@@ -30768,7 +30822,7 @@
       <c r="I955" s="46"/>
       <c r="J955" s="73"/>
     </row>
-    <row r="956" spans="1:11" ht="13.2">
+    <row r="956" spans="1:13" ht="13.2">
       <c r="A956" s="19">
         <v>155</v>
       </c>
@@ -30789,7 +30843,7 @@
       <c r="I956" s="46"/>
       <c r="J956" s="73"/>
     </row>
-    <row r="957" spans="1:11" ht="52.8">
+    <row r="957" spans="1:13" ht="52.8">
       <c r="A957" s="19">
         <v>155</v>
       </c>
@@ -30810,10 +30864,10 @@
       <c r="I957" s="46"/>
       <c r="J957" s="73"/>
       <c r="K957" s="82" t="s">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="958" spans="1:11" ht="26.4">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="958" spans="1:13" ht="92.4">
       <c r="A958" s="19">
         <v>155</v>
       </c>
@@ -30835,11 +30889,17 @@
       <c r="H958" s="46"/>
       <c r="I958" s="46"/>
       <c r="J958" s="73"/>
-      <c r="K958" s="82" t="s">
+      <c r="K958" s="83" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="959" spans="1:11" ht="13.2">
+      <c r="L958" s="82" t="s">
+        <v>1045</v>
+      </c>
+      <c r="M958" s="82" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="959" spans="1:13" ht="13.2">
       <c r="A959" s="19">
         <v>155</v>
       </c>
@@ -30860,7 +30920,7 @@
       <c r="I959" s="46"/>
       <c r="J959" s="73"/>
     </row>
-    <row r="960" spans="1:11" ht="13.2">
+    <row r="960" spans="1:13" ht="13.2">
       <c r="A960" s="19">
         <v>155</v>
       </c>
@@ -30881,7 +30941,7 @@
       <c r="I960" s="46"/>
       <c r="J960" s="73"/>
     </row>
-    <row r="961" spans="1:11" ht="13.2">
+    <row r="961" spans="1:13" ht="13.2">
       <c r="A961" s="19">
         <v>155</v>
       </c>
@@ -30902,7 +30962,7 @@
       <c r="I961" s="46"/>
       <c r="J961" s="73"/>
     </row>
-    <row r="962" spans="1:11" ht="13.2">
+    <row r="962" spans="1:13" ht="13.2">
       <c r="A962" s="19">
         <v>155</v>
       </c>
@@ -30923,7 +30983,7 @@
       <c r="I962" s="46"/>
       <c r="J962" s="73"/>
     </row>
-    <row r="963" spans="1:11" ht="26.4">
+    <row r="963" spans="1:13" ht="26.4">
       <c r="A963" s="19">
         <v>155</v>
       </c>
@@ -30946,10 +31006,10 @@
       <c r="I963" s="46"/>
       <c r="J963" s="73"/>
       <c r="K963" s="82" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="964" spans="1:11" ht="13.2">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="964" spans="1:13" ht="13.2">
       <c r="A964" s="19">
         <v>157</v>
       </c>
@@ -30970,7 +31030,7 @@
       <c r="I964" s="36"/>
       <c r="J964" s="71"/>
     </row>
-    <row r="965" spans="1:11" ht="13.2">
+    <row r="965" spans="1:13" ht="13.2">
       <c r="A965" s="19">
         <v>157</v>
       </c>
@@ -30991,7 +31051,7 @@
       <c r="I965" s="36"/>
       <c r="J965" s="71"/>
     </row>
-    <row r="966" spans="1:11" ht="13.2">
+    <row r="966" spans="1:13" ht="13.2">
       <c r="A966" s="19">
         <v>157</v>
       </c>
@@ -31012,7 +31072,7 @@
       <c r="I966" s="36"/>
       <c r="J966" s="71"/>
     </row>
-    <row r="967" spans="1:11" ht="13.2">
+    <row r="967" spans="1:13" ht="13.2">
       <c r="A967" s="19">
         <v>157</v>
       </c>
@@ -31033,7 +31093,7 @@
       <c r="I967" s="36"/>
       <c r="J967" s="71"/>
     </row>
-    <row r="968" spans="1:11" ht="13.2">
+    <row r="968" spans="1:13" ht="13.2">
       <c r="A968" s="19">
         <v>157</v>
       </c>
@@ -31054,7 +31114,7 @@
       <c r="I968" s="36"/>
       <c r="J968" s="71"/>
     </row>
-    <row r="969" spans="1:11" ht="13.2">
+    <row r="969" spans="1:13" ht="13.2">
       <c r="A969" s="19">
         <v>157</v>
       </c>
@@ -31075,7 +31135,7 @@
       <c r="I969" s="36"/>
       <c r="J969" s="71"/>
     </row>
-    <row r="970" spans="1:11" ht="13.2">
+    <row r="970" spans="1:13" ht="13.2">
       <c r="A970" s="19">
         <v>157</v>
       </c>
@@ -31096,7 +31156,7 @@
       <c r="I970" s="36"/>
       <c r="J970" s="71"/>
     </row>
-    <row r="971" spans="1:11" ht="13.2">
+    <row r="971" spans="1:13" ht="13.2">
       <c r="A971" s="19">
         <v>157</v>
       </c>
@@ -31117,7 +31177,7 @@
       <c r="I971" s="36"/>
       <c r="J971" s="71"/>
     </row>
-    <row r="972" spans="1:11" ht="13.2">
+    <row r="972" spans="1:13" ht="13.2">
       <c r="A972" s="19">
         <v>157</v>
       </c>
@@ -31138,7 +31198,7 @@
       <c r="I972" s="36"/>
       <c r="J972" s="71"/>
     </row>
-    <row r="973" spans="1:11" ht="13.2">
+    <row r="973" spans="1:13" ht="13.2">
       <c r="A973" s="19">
         <v>157</v>
       </c>
@@ -31159,7 +31219,7 @@
       <c r="I973" s="36"/>
       <c r="J973" s="71"/>
     </row>
-    <row r="974" spans="1:11" ht="26.4">
+    <row r="974" spans="1:13" ht="26.4">
       <c r="A974" s="19">
         <v>160</v>
       </c>
@@ -31182,10 +31242,10 @@
       <c r="I974" s="46"/>
       <c r="J974" s="73"/>
       <c r="K974" s="82" t="s">
-        <v>962</v>
-      </c>
-    </row>
-    <row r="975" spans="1:11" ht="39.6">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="975" spans="1:13" ht="52.8">
       <c r="A975" s="19">
         <v>160</v>
       </c>
@@ -31210,8 +31270,14 @@
       <c r="K975" s="82" t="s">
         <v>929</v>
       </c>
-    </row>
-    <row r="976" spans="1:11" ht="13.2">
+      <c r="L975" s="82" t="s">
+        <v>1046</v>
+      </c>
+      <c r="M975" s="82" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="976" spans="1:13" ht="13.2">
       <c r="A976" s="19">
         <v>160</v>
       </c>
@@ -31316,7 +31382,7 @@
       <c r="I980" s="46"/>
       <c r="J980" s="73"/>
     </row>
-    <row r="981" spans="1:11" ht="39.6">
+    <row r="981" spans="1:11" ht="26.4">
       <c r="A981" s="19">
         <v>160</v>
       </c>
@@ -31339,7 +31405,7 @@
       <c r="I981" s="46"/>
       <c r="J981" s="73"/>
       <c r="K981" s="82" t="s">
-        <v>963</v>
+        <v>915</v>
       </c>
     </row>
     <row r="982" spans="1:11" ht="13.2">
@@ -31619,7 +31685,7 @@
       <c r="I994" s="46"/>
       <c r="J994" s="73"/>
       <c r="K994" s="82" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
     </row>
     <row r="995" spans="1:11" ht="26.4">
@@ -31709,8 +31775,8 @@
       <c r="H998" s="46"/>
       <c r="I998" s="46"/>
       <c r="J998" s="73"/>
-      <c r="K998" s="82" t="s">
-        <v>965</v>
+      <c r="K998" s="83" t="s">
+        <v>963</v>
       </c>
     </row>
     <row r="999" spans="1:11" ht="26.4">
@@ -31736,7 +31802,7 @@
       <c r="I999" s="46"/>
       <c r="J999" s="73"/>
       <c r="K999" s="82" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
     </row>
     <row r="1000" spans="1:11" ht="26.4">
@@ -31832,7 +31898,7 @@
       <c r="I1003" s="36"/>
       <c r="J1003" s="71"/>
       <c r="K1003" s="82" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
     </row>
     <row r="1004" spans="1:11" ht="13.2">
@@ -31860,7 +31926,7 @@
       <c r="I1004" s="36"/>
       <c r="J1004" s="71"/>
       <c r="K1004" s="82" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
     </row>
     <row r="1005" spans="1:11" ht="26.4">
@@ -31886,7 +31952,7 @@
       <c r="I1005" s="36"/>
       <c r="J1005" s="71"/>
       <c r="K1005" s="82" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
     </row>
     <row r="1006" spans="1:11" ht="13.2">
@@ -32185,7 +32251,7 @@
       <c r="I1019" s="36"/>
       <c r="J1019" s="71"/>
       <c r="K1019" s="82" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
     </row>
     <row r="1020" spans="1:11" ht="26.4">
@@ -32213,7 +32279,7 @@
       <c r="I1020" s="36"/>
       <c r="J1020" s="71"/>
       <c r="K1020" s="82" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
     </row>
     <row r="1021" spans="1:11" ht="26.4">
@@ -32309,7 +32375,7 @@
       <c r="I1024" s="36"/>
       <c r="J1024" s="71"/>
       <c r="K1024" s="82" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
     </row>
     <row r="1025" spans="1:11" ht="26.4">
@@ -32419,7 +32485,7 @@
       <c r="I1029" s="46"/>
       <c r="J1029" s="73"/>
       <c r="K1029" s="82" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="1030" spans="1:11" ht="13.2">
@@ -32468,7 +32534,7 @@
       <c r="I1031" s="46"/>
       <c r="J1031" s="73"/>
       <c r="K1031" s="82" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
     </row>
     <row r="1032" spans="1:11" ht="13.2">
@@ -32557,7 +32623,7 @@
       <c r="I1035" s="46"/>
       <c r="J1035" s="73"/>
       <c r="K1035" s="82" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
     </row>
     <row r="1036" spans="1:11" ht="13.2">
@@ -32686,7 +32752,7 @@
       <c r="I1041" s="36"/>
       <c r="J1041" s="71"/>
       <c r="K1041" s="82" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
     </row>
     <row r="1042" spans="1:11" ht="26.4">
@@ -32862,7 +32928,7 @@
       <c r="I1049" s="46"/>
       <c r="J1049" s="73"/>
       <c r="K1049" s="82" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
     </row>
     <row r="1050" spans="1:11" ht="13.2">
@@ -32928,7 +32994,7 @@
       <c r="I1052" s="46"/>
       <c r="J1052" s="73"/>
       <c r="K1052" s="82" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
     </row>
     <row r="1053" spans="1:11" ht="13.2">
@@ -33038,7 +33104,7 @@
       <c r="I1057" s="36"/>
       <c r="J1057" s="71"/>
       <c r="K1057" s="82" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="1058" spans="1:11" ht="13.2">
@@ -33083,7 +33149,7 @@
       <c r="I1059" s="36"/>
       <c r="J1059" s="71"/>
       <c r="K1059" s="82" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
     </row>
     <row r="1060" spans="1:11" ht="26.4">
@@ -33107,7 +33173,7 @@
       <c r="I1060" s="36"/>
       <c r="J1060" s="71"/>
       <c r="K1060" s="82" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
     </row>
     <row r="1061" spans="1:11" ht="13.2">
@@ -33154,7 +33220,7 @@
       <c r="I1062" s="36"/>
       <c r="J1062" s="71"/>
       <c r="K1062" s="82" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
     </row>
     <row r="1063" spans="1:11" ht="13.2">
@@ -33220,7 +33286,7 @@
       <c r="I1065" s="36"/>
       <c r="J1065" s="71"/>
       <c r="K1065" s="82" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
     </row>
     <row r="1066" spans="1:11" ht="26.4">
@@ -33391,7 +33457,7 @@
       <c r="I1073" s="46"/>
       <c r="J1073" s="73"/>
       <c r="K1073" s="82" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="1074" spans="1:11" ht="26.4">
@@ -33438,7 +33504,7 @@
       <c r="I1075" s="36"/>
       <c r="J1075" s="71"/>
       <c r="K1075" s="82" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
     </row>
     <row r="1076" spans="1:11" ht="13.2">
@@ -33527,7 +33593,7 @@
       <c r="I1079" s="36"/>
       <c r="J1079" s="71"/>
       <c r="K1079" s="82" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
     </row>
     <row r="1080" spans="1:11" ht="13.2">
@@ -33614,7 +33680,7 @@
       <c r="I1083" s="36"/>
       <c r="J1083" s="71"/>
       <c r="K1083" s="82" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
     </row>
     <row r="1084" spans="1:11" ht="13.2">
@@ -33682,7 +33748,7 @@
       <c r="I1086" s="46"/>
       <c r="J1086" s="73"/>
       <c r="K1086" s="82" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="1087" spans="1:11" ht="13.2">
@@ -33752,7 +33818,7 @@
       <c r="I1089" s="46"/>
       <c r="J1089" s="73"/>
       <c r="K1089" s="82" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
     </row>
     <row r="1090" spans="1:11" ht="13.2">
@@ -33799,7 +33865,7 @@
       <c r="I1091" s="46"/>
       <c r="J1091" s="73"/>
       <c r="K1091" s="82" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
     </row>
     <row r="1092" spans="1:11" ht="79.2">
@@ -33823,7 +33889,7 @@
       <c r="I1092" s="46"/>
       <c r="J1092" s="73"/>
       <c r="K1092" s="82" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
     </row>
     <row r="1093" spans="1:11" ht="13.2">
@@ -33933,7 +33999,7 @@
       <c r="I1097" s="36"/>
       <c r="J1097" s="71"/>
       <c r="K1097" s="82" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="1098" spans="1:11" ht="105.6">
@@ -33959,7 +34025,7 @@
       <c r="I1098" s="36"/>
       <c r="J1098" s="71"/>
       <c r="K1098" s="82" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
     </row>
     <row r="1099" spans="1:11" ht="39.6">
@@ -33985,7 +34051,7 @@
       <c r="I1099" s="36"/>
       <c r="J1099" s="71"/>
       <c r="K1099" s="82" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="1100" spans="1:11" ht="13.2">
@@ -34114,7 +34180,7 @@
       <c r="I1105" s="46"/>
       <c r="J1105" s="73"/>
       <c r="K1105" s="82" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="1106" spans="1:11" ht="13.2">
@@ -34184,7 +34250,7 @@
       <c r="I1108" s="46"/>
       <c r="J1108" s="73"/>
       <c r="K1108" s="82" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
     </row>
     <row r="1109" spans="1:11" ht="13.2">
@@ -34451,7 +34517,7 @@
       <c r="I1120" s="36"/>
       <c r="J1120" s="71"/>
       <c r="K1120" s="82" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
     </row>
     <row r="1121" spans="1:11" ht="13.2">
@@ -34543,7 +34609,7 @@
       <c r="I1124" s="46"/>
       <c r="J1124" s="73"/>
       <c r="K1124" s="82" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="1125" spans="1:11" ht="13.2">
@@ -34632,7 +34698,7 @@
       <c r="I1128" s="46"/>
       <c r="J1128" s="73"/>
       <c r="K1128" s="82" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="1129" spans="1:11" ht="13.2">
@@ -34843,7 +34909,7 @@
       <c r="I1138" s="36"/>
       <c r="J1138" s="71"/>
       <c r="K1138" s="82" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
     </row>
     <row r="1139" spans="1:11" ht="13.2">
@@ -34955,7 +35021,7 @@
       <c r="I1143" s="46"/>
       <c r="J1143" s="73"/>
       <c r="K1143" s="82" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
     </row>
     <row r="1144" spans="1:11" ht="26.4">
@@ -35044,7 +35110,7 @@
       <c r="I1147" s="46"/>
       <c r="J1147" s="73"/>
       <c r="K1147" s="82" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
     <row r="1148" spans="1:11" ht="26.4">
@@ -35154,7 +35220,7 @@
       <c r="I1152" s="36"/>
       <c r="J1152" s="71"/>
       <c r="K1152" s="82" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
     </row>
     <row r="1153" spans="1:11" ht="26.4">
@@ -35648,10 +35714,10 @@
       <c r="I1175" s="36"/>
       <c r="J1175" s="71"/>
       <c r="K1175" s="82" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="L1175" s="82" t="s">
-        <v>1035</v>
+        <v>1032</v>
       </c>
       <c r="M1175" s="82" t="s">
         <v>738</v>
@@ -35701,7 +35767,7 @@
       <c r="I1177" s="46"/>
       <c r="J1177" s="73"/>
       <c r="K1177" s="82" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
     </row>
     <row r="1178" spans="1:13" ht="39.6">
@@ -35727,7 +35793,7 @@
       <c r="I1178" s="46"/>
       <c r="J1178" s="73"/>
       <c r="K1178" s="82" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
     </row>
     <row r="1179" spans="1:13" ht="39.6">
@@ -35753,7 +35819,7 @@
       <c r="I1179" s="46"/>
       <c r="J1179" s="73"/>
       <c r="K1179" s="82" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="1180" spans="1:13" ht="26.4">
@@ -35800,7 +35866,7 @@
       <c r="I1181" s="46"/>
       <c r="J1181" s="73"/>
       <c r="K1181" s="82" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
     </row>
     <row r="1182" spans="1:13" ht="26.4">
@@ -35953,7 +36019,7 @@
       <c r="I1188" s="36"/>
       <c r="J1188" s="71"/>
       <c r="K1188" s="82" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
     </row>
     <row r="1189" spans="1:11" ht="13.2">
@@ -36126,7 +36192,7 @@
       <c r="I1196" s="46"/>
       <c r="J1196" s="73"/>
       <c r="K1196" s="82" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
     </row>
     <row r="1197" spans="1:11" ht="13.2">
@@ -36381,7 +36447,7 @@
       <c r="I1208" s="36"/>
       <c r="J1208" s="71"/>
       <c r="K1208" s="82" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="1209" spans="1:11" ht="26.4">
@@ -36512,7 +36578,7 @@
       <c r="I1214" s="46"/>
       <c r="J1214" s="73"/>
       <c r="K1214" s="82" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
     </row>
     <row r="1215" spans="1:11" ht="13.2">
@@ -36580,7 +36646,7 @@
       <c r="I1217" s="46"/>
       <c r="J1217" s="73"/>
       <c r="K1217" s="82" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
     </row>
     <row r="1218" spans="1:11" ht="13.2">
@@ -36812,7 +36878,7 @@
       <c r="I1228" s="36"/>
       <c r="J1228" s="71"/>
       <c r="K1228" s="82" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="1229" spans="1:11" ht="13.2">
@@ -36943,7 +37009,7 @@
       <c r="I1234" s="46"/>
       <c r="J1234" s="73"/>
       <c r="K1234" s="82" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="1235" spans="1:11" ht="13.2">
@@ -37200,7 +37266,7 @@
       <c r="I1246" s="36"/>
       <c r="J1246" s="71"/>
       <c r="K1246" s="82" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="1247" spans="1:11" ht="13.2">
@@ -37518,7 +37584,7 @@
       <c r="I1261" s="36"/>
       <c r="J1261" s="71"/>
       <c r="K1261" s="82" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
     </row>
     <row r="1262" spans="1:11" ht="13.2">
@@ -37565,7 +37631,7 @@
       <c r="I1263" s="36"/>
       <c r="J1263" s="71"/>
       <c r="K1263" s="82" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="1264" spans="1:11" ht="13.2">
@@ -37637,7 +37703,7 @@
       <c r="I1266" s="36"/>
       <c r="J1266" s="71"/>
       <c r="K1266" s="82" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="1267" spans="1:11" ht="13.2">
@@ -37705,7 +37771,7 @@
       <c r="I1269" s="46"/>
       <c r="J1269" s="73"/>
       <c r="K1269" s="82" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="1270" spans="1:11" ht="13.2">
@@ -37773,7 +37839,7 @@
       <c r="I1272" s="46"/>
       <c r="J1272" s="73"/>
       <c r="K1272" s="82" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="1273" spans="1:11" ht="13.2">
@@ -37867,7 +37933,7 @@
       <c r="I1276" s="36"/>
       <c r="J1276" s="71"/>
       <c r="K1276" s="82" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="1277" spans="1:11" ht="26.4">
@@ -37933,7 +37999,7 @@
       <c r="I1279" s="36"/>
       <c r="J1279" s="71"/>
       <c r="K1279" s="82" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="1280" spans="1:11" ht="26.4">
@@ -38386,7 +38452,7 @@
       <c r="I1300" s="36"/>
       <c r="J1300" s="71"/>
       <c r="K1300" s="82" t="s">
-        <v>1011</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="1301" spans="1:11" ht="52.8">

</xml_diff>

<commit_message>
edited OOSTT user-centered definition: trauma quality improvement and patient safety program lead role
</commit_message>
<xml_diff>
--- a/TermSurveyResponses.xlsx
+++ b/TermSurveyResponses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathiasbrochhausen/OOSTT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB688755-637B-C742-9364-842A60669C6C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35ED0C3-2A4D-BD45-8536-F1E2535C600E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="3420" windowWidth="33280" windowHeight="17040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1060" yWindow="960" windowWidth="27740" windowHeight="17040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="1021">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="1024">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -3130,6 +3130,15 @@
   </si>
   <si>
     <t xml:space="preserve">Ask Mathias: should we providemore description of the expectation? </t>
+  </si>
+  <si>
+    <t>added a CAFÉ application label "trauma nursing evaluator"</t>
+  </si>
+  <si>
+    <t>The role of a healthcare provider that ensures trauma quality improvement and patient safety within the trauma program.</t>
+  </si>
+  <si>
+    <t>edited OOSTT definition</t>
   </si>
 </sst>
 </file>
@@ -9534,8 +9543,8 @@
   <dimension ref="A1:IW1418"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A478" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B367" sqref="B367"/>
+      <pane ySplit="1" topLeftCell="A445" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H452" sqref="H452:H461"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -19475,7 +19484,7 @@
       <c r="E452" s="45"/>
       <c r="F452" s="46"/>
       <c r="G452" s="47"/>
-      <c r="H452" s="47"/>
+      <c r="H452" s="60"/>
       <c r="I452" s="47"/>
       <c r="J452" s="47"/>
     </row>
@@ -19496,7 +19505,7 @@
       <c r="E453" s="45"/>
       <c r="F453" s="46"/>
       <c r="G453" s="47"/>
-      <c r="H453" s="47"/>
+      <c r="H453" s="60"/>
       <c r="I453" s="47"/>
       <c r="J453" s="47"/>
     </row>
@@ -19515,7 +19524,7 @@
       <c r="E454" s="45"/>
       <c r="F454" s="46"/>
       <c r="G454" s="47"/>
-      <c r="H454" s="47"/>
+      <c r="H454" s="60"/>
       <c r="I454" s="47"/>
       <c r="J454" s="47"/>
     </row>
@@ -19540,7 +19549,7 @@
         <v>264</v>
       </c>
       <c r="G455" s="47"/>
-      <c r="H455" s="47"/>
+      <c r="H455" s="60"/>
       <c r="I455" s="47"/>
       <c r="J455" s="47"/>
     </row>
@@ -19563,7 +19572,7 @@
       </c>
       <c r="F456" s="46"/>
       <c r="G456" s="47"/>
-      <c r="H456" s="47"/>
+      <c r="H456" s="60"/>
       <c r="I456" s="47"/>
       <c r="J456" s="47"/>
     </row>
@@ -19585,8 +19594,10 @@
       <c r="F457" s="55" t="s">
         <v>266</v>
       </c>
-      <c r="G457" s="47"/>
-      <c r="H457" s="47"/>
+      <c r="G457" s="47" t="s">
+        <v>1021</v>
+      </c>
+      <c r="H457" s="60"/>
       <c r="I457" s="47"/>
       <c r="J457" s="47"/>
       <c r="K457" s="8" t="s">
@@ -19610,7 +19621,7 @@
         <v>267</v>
       </c>
       <c r="G458" s="47"/>
-      <c r="H458" s="47"/>
+      <c r="H458" s="60"/>
       <c r="I458" s="47"/>
       <c r="J458" s="47"/>
     </row>
@@ -19629,7 +19640,7 @@
       <c r="E459" s="45"/>
       <c r="F459" s="46"/>
       <c r="G459" s="47"/>
-      <c r="H459" s="47"/>
+      <c r="H459" s="60"/>
       <c r="I459" s="47"/>
       <c r="J459" s="47"/>
     </row>
@@ -19654,7 +19665,7 @@
         <v>269</v>
       </c>
       <c r="G460" s="47"/>
-      <c r="H460" s="47"/>
+      <c r="H460" s="60"/>
       <c r="I460" s="47"/>
       <c r="J460" s="47"/>
     </row>
@@ -19677,7 +19688,7 @@
       </c>
       <c r="F461" s="46"/>
       <c r="G461" s="47"/>
-      <c r="H461" s="47"/>
+      <c r="H461" s="60"/>
       <c r="I461" s="47"/>
       <c r="J461" s="47"/>
       <c r="K461" s="8" t="s">
@@ -31916,9 +31927,13 @@
       <c r="F1019" s="57" t="s">
         <v>403</v>
       </c>
-      <c r="G1019" s="36"/>
-      <c r="H1019" s="36"/>
-      <c r="I1019" s="36"/>
+      <c r="G1019" s="36" t="s">
+        <v>1023</v>
+      </c>
+      <c r="H1019" s="60"/>
+      <c r="I1019" s="36" t="s">
+        <v>1022</v>
+      </c>
       <c r="J1019" s="36"/>
       <c r="K1019" s="8" t="s">
         <v>977</v>
@@ -31945,7 +31960,7 @@
         <v>405</v>
       </c>
       <c r="G1020" s="36"/>
-      <c r="H1020" s="36"/>
+      <c r="H1020" s="60"/>
       <c r="I1020" s="36"/>
       <c r="J1020" s="36"/>
       <c r="K1020" s="8" t="s">
@@ -31971,7 +31986,7 @@
       </c>
       <c r="F1021" s="37"/>
       <c r="G1021" s="36"/>
-      <c r="H1021" s="36"/>
+      <c r="H1021" s="60"/>
       <c r="I1021" s="36"/>
       <c r="J1021" s="36"/>
     </row>
@@ -31994,7 +32009,7 @@
         <v>407</v>
       </c>
       <c r="G1022" s="36"/>
-      <c r="H1022" s="36"/>
+      <c r="H1022" s="60"/>
       <c r="I1022" s="36"/>
       <c r="J1022" s="36"/>
       <c r="K1022" s="8" t="s">
@@ -32018,7 +32033,7 @@
       <c r="E1023" s="56"/>
       <c r="F1023" s="37"/>
       <c r="G1023" s="36"/>
-      <c r="H1023" s="36"/>
+      <c r="H1023" s="60"/>
       <c r="I1023" s="36"/>
       <c r="J1023" s="36"/>
     </row>
@@ -32041,7 +32056,7 @@
         <v>408</v>
       </c>
       <c r="G1024" s="36"/>
-      <c r="H1024" s="36"/>
+      <c r="H1024" s="60"/>
       <c r="I1024" s="36"/>
       <c r="J1024" s="36"/>
       <c r="K1024" s="8" t="s">
@@ -32065,7 +32080,7 @@
       <c r="E1025" s="56"/>
       <c r="F1025" s="37"/>
       <c r="G1025" s="36"/>
-      <c r="H1025" s="36"/>
+      <c r="H1025" s="60"/>
       <c r="I1025" s="36"/>
       <c r="J1025" s="36"/>
     </row>
@@ -32086,7 +32101,7 @@
       <c r="E1026" s="56"/>
       <c r="F1026" s="37"/>
       <c r="G1026" s="36"/>
-      <c r="H1026" s="36"/>
+      <c r="H1026" s="60"/>
       <c r="I1026" s="36"/>
       <c r="J1026" s="36"/>
     </row>
@@ -32107,7 +32122,7 @@
       <c r="E1027" s="56"/>
       <c r="F1027" s="37"/>
       <c r="G1027" s="36"/>
-      <c r="H1027" s="36"/>
+      <c r="H1027" s="60"/>
       <c r="I1027" s="36"/>
       <c r="J1027" s="36"/>
     </row>

</xml_diff>